<commit_message>
Corrected DSP Channel in DataSet
</commit_message>
<xml_diff>
--- a/AutoFirmwareUpgrade/ClassLibrary1/TestDataFiles/CablingDataSet/1U4U3I3I3I.xlsx
+++ b/AutoFirmwareUpgrade/ClassLibrary1/TestDataFiles/CablingDataSet/1U4U3I3I3I.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534D8BEC-2ACA-4253-83DF-619DC04F3ED9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9BF04EC-22D1-4630-89EB-15DEC37B238D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -624,7 +624,7 @@
   <dimension ref="A1:AB23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:J4"/>
+      <selection activeCell="B14" sqref="B14:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1426,7 +1426,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1554,7 +1554,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C9">
         <v>7</v>
@@ -1568,7 +1568,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C10">
         <v>8</v>
@@ -1582,7 +1582,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C11">
         <v>9</v>
@@ -1596,7 +1596,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C12">
         <v>10</v>

</xml_diff>